<commit_message>
Arreglando check rfc y descuento
Arreglando check rfc y descuento
</commit_message>
<xml_diff>
--- a/019-085-WENDLANDT-VENTAS/src/WendlandtVentas.Web/wwwroot/resources/Facturación Wendlandt.xlsx
+++ b/019-085-WENDLANDT-VENTAS/src/WendlandtVentas.Web/wwwroot/resources/Facturación Wendlandt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\WEND-Ventas\019-085-WENDLANDT-VENTAS\src\WendlandtVentas.Web\wwwroot\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Viera\Documents\GitHub\Wend-Sys\019-085-WENDLANDT-VENTAS\src\WendlandtVentas.Web\wwwroot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830B4458-591D-453D-B4B9-1BCCF9D46CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0245F16E-CEFC-445B-92AD-CF499F4B3FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{1F49A7E6-679B-4399-A417-11073B80C7DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F49A7E6-679B-4399-A417-11073B80C7DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t xml:space="preserve">Nombre:  </t>
   </si>
   <si>
-    <t>Firma recepción</t>
-  </si>
-  <si>
     <t>Firma entrega</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>PESO NETO</t>
+  </si>
+  <si>
+    <t>Firma, nombre y fecha de recepción</t>
   </si>
 </sst>
 </file>
@@ -129,7 +129,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -314,9 +314,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -325,65 +325,85 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -395,66 +415,45 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,9 +573,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -614,7 +613,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -720,7 +719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -862,7 +861,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -872,23 +871,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B3F7D2-6CB9-428A-A4C2-146A1DE2B743}">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14:T26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.77734375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="2.21875" style="1" customWidth="1"/>
     <col min="8" max="10" width="5.77734375" style="1" customWidth="1"/>
     <col min="11" max="11" width="7.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.77734375" style="1" customWidth="1"/>
-    <col min="14" max="15" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="11.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="1"/>
     <col min="16" max="16" width="7.77734375" style="1" customWidth="1"/>
     <col min="17" max="17" width="2.21875" style="1" customWidth="1"/>
     <col min="18" max="20" width="5.77734375" style="1" customWidth="1"/>
@@ -912,181 +913,181 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="38"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="18" t="s">
+      <c r="R2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="19"/>
-      <c r="T2" s="20"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="38"/>
     </row>
     <row r="3" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="21">
+      <c r="H3" s="39">
         <v>5932</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="41"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="21">
+      <c r="R3" s="39">
         <v>5932</v>
       </c>
-      <c r="S3" s="22"/>
-      <c r="T3" s="23"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="41"/>
     </row>
     <row r="4" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
+      <c r="H4" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="30" t="s">
+      <c r="N4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="16"/>
-      <c r="T4" s="17"/>
+      <c r="R4" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="43"/>
+      <c r="T4" s="44"/>
     </row>
     <row r="5" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="21">
+      <c r="H5" s="39">
         <v>2020000033</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="41"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="21">
+      <c r="R5" s="39">
         <v>2020000033</v>
       </c>
-      <c r="S5" s="22"/>
-      <c r="T5" s="23"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="41"/>
     </row>
     <row r="6" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="32" t="s">
+      <c r="R6" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
     </row>
     <row r="7" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7" s="8" t="s">
+      <c r="R7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="T7" s="8" t="s">
+      <c r="T7" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1113,82 +1114,82 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A9" s="4"/>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
-      <c r="L9" s="27" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+      <c r="L9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="29"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="35"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A10" s="4"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="29"/>
-      <c r="L10" s="27" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
+      <c r="L10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="29"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="35"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A11" s="4"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="29"/>
-      <c r="L11" s="27" t="s">
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="L11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28" t="s">
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="28"/>
-      <c r="T11" s="29"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="35"/>
     </row>
     <row r="12" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4"/>
@@ -1213,420 +1214,420 @@
     </row>
     <row r="13" spans="1:20" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4"/>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="33" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="24" t="s">
+      <c r="H13" s="31"/>
+      <c r="I13" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="26"/>
-      <c r="L13" s="7" t="s">
+      <c r="J13" s="28"/>
+      <c r="L13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="M13" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="33" t="s">
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="R13" s="34"/>
-      <c r="S13" s="24" t="s">
+      <c r="R13" s="31"/>
+      <c r="S13" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="T13" s="26"/>
+      <c r="T13" s="28"/>
     </row>
     <row r="14" spans="1:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="48"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="48"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="15"/>
     </row>
     <row r="15" spans="1:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="48"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="46"/>
-      <c r="S15" s="47"/>
-      <c r="T15" s="48"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="15"/>
     </row>
     <row r="16" spans="1:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="48"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="47"/>
-      <c r="T16" s="48"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="15"/>
     </row>
     <row r="17" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="48"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="46"/>
-      <c r="S17" s="47"/>
-      <c r="T17" s="48"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="15"/>
     </row>
     <row r="18" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="48"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="47"/>
-      <c r="T18" s="48"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="15"/>
     </row>
     <row r="19" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="48"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="46"/>
-      <c r="S19" s="47"/>
-      <c r="T19" s="48"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="15"/>
     </row>
     <row r="20" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B20" s="3"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="48"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="46"/>
-      <c r="S20" s="47"/>
-      <c r="T20" s="48"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="15"/>
     </row>
     <row r="21" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="46"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="48"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="15"/>
     </row>
     <row r="22" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="48"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="46"/>
-      <c r="S22" s="47"/>
-      <c r="T22" s="48"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="15"/>
     </row>
     <row r="23" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="48"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="47"/>
-      <c r="T23" s="48"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="15"/>
     </row>
     <row r="24" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="48"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="45"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="47"/>
-      <c r="T24" s="48"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="15"/>
     </row>
     <row r="25" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="48"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="47"/>
-      <c r="T25" s="48"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="15"/>
     </row>
     <row r="26" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="15"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="46"/>
-      <c r="S26" s="47"/>
-      <c r="T26" s="48"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="15"/>
     </row>
     <row r="27" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="L27" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="21"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="R27" s="18"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+    </row>
+    <row r="28" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R28" s="18"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+    </row>
+    <row r="29" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B29" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="40"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="L27" s="11" t="s">
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="L29" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="M27" s="11"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="R27" s="40"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-    </row>
-    <row r="28" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="42"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="39"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="R28" s="40"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="43"/>
-    </row>
-    <row r="29" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
+      <c r="M29" s="21"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R29" s="18"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+    </row>
+    <row r="30" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="20"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="25"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="R30" s="20"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+    </row>
+    <row r="31" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B31" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="L29" s="11" t="s">
+      <c r="C31" s="21"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="L31" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="11"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="R29" s="40"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="43"/>
-    </row>
-    <row r="30" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="37"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="39"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="R30" s="37"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-    </row>
-    <row r="31" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="L31" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31" s="11"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
     </row>
     <row r="32" spans="2:20" ht="43.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G32" s="5"/>
@@ -1639,32 +1640,32 @@
       <c r="T32" s="5"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="B33" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="6"/>
+      <c r="B33" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="L33" s="35" t="s">
+      <c r="H33" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="6"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="L33" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
-      <c r="R33" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="S33" s="35"/>
-      <c r="T33" s="35"/>
+      <c r="R33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
     </row>
     <row r="34" spans="2:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="35" spans="2:20" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1692,6 +1693,128 @@
     <row r="64" ht="8.4" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="146">
+    <mergeCell ref="N29:P30"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="D27:F28"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="D29:F30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B9:J9"/>
+    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="L9:T9"/>
+    <mergeCell ref="L10:T10"/>
+    <mergeCell ref="L11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
     <mergeCell ref="L33:N33"/>
     <mergeCell ref="R33:T33"/>
     <mergeCell ref="M26:P26"/>
@@ -1716,128 +1839,6 @@
     <mergeCell ref="L29:M30"/>
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="N27:P28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="L9:T9"/>
-    <mergeCell ref="L10:T10"/>
-    <mergeCell ref="L11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B9:J9"/>
-    <mergeCell ref="B10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="N29:P30"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="D27:F28"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="D29:F30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="M22:P22"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion plantillas remision y factura
</commit_message>
<xml_diff>
--- a/019-085-WENDLANDT-VENTAS/src/WendlandtVentas.Web/wwwroot/resources/Facturación Wendlandt.xlsx
+++ b/019-085-WENDLANDT-VENTAS/src/WendlandtVentas.Web/wwwroot/resources/Facturación Wendlandt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Viera\Documents\GitHub\Wend-Sys\019-085-WENDLANDT-VENTAS\src\WendlandtVentas.Web\wwwroot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0245F16E-CEFC-445B-92AD-CF499F4B3FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D096B46-0D1C-45E1-98A2-2FA6747BFB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F49A7E6-679B-4399-A417-11073B80C7DF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>CANT</t>
   </si>
@@ -103,9 +103,6 @@
     <t xml:space="preserve">Nombre:  </t>
   </si>
   <si>
-    <t>Firma entrega</t>
-  </si>
-  <si>
     <t>DIA</t>
   </si>
   <si>
@@ -121,7 +118,16 @@
     <t>PESO NETO</t>
   </si>
   <si>
-    <t>Firma, nombre y fecha de recepción</t>
+    <t>Firma</t>
+  </si>
+  <si>
+    <t>Nombre Completo</t>
+  </si>
+  <si>
+    <t>Fecha de recepcion</t>
+  </si>
+  <si>
+    <t>Fecha de entrega</t>
   </si>
 </sst>
 </file>
@@ -131,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +196,19 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -211,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -302,15 +321,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -331,7 +341,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -349,106 +367,94 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -869,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B3F7D2-6CB9-428A-A4C2-146A1DE2B743}">
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -913,159 +919,159 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="36" t="s">
+      <c r="R2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="37"/>
-      <c r="T2" s="38"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="23"/>
     </row>
     <row r="3" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="39">
+      <c r="H3" s="24">
         <v>5932</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="23" t="s">
+      <c r="N3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="39">
+      <c r="R3" s="24">
         <v>5932</v>
       </c>
-      <c r="S3" s="40"/>
-      <c r="T3" s="41"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="26"/>
     </row>
     <row r="4" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="H4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="43"/>
-      <c r="T4" s="44"/>
+      <c r="R4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="19"/>
+      <c r="T4" s="20"/>
     </row>
     <row r="5" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="39">
+      <c r="H5" s="24">
         <v>2020000033</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="41"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="39">
+      <c r="R5" s="24">
         <v>2020000033</v>
       </c>
-      <c r="S5" s="40"/>
-      <c r="T5" s="41"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="26"/>
     </row>
     <row r="6" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="45" t="s">
+      <c r="H6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="45" t="s">
+      <c r="R6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
     </row>
     <row r="7" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="4"/>
       <c r="H7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>5</v>
@@ -1075,14 +1081,14 @@
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="32" t="s">
+      <c r="N7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>5</v>
@@ -1114,82 +1120,82 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A9" s="4"/>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="35"/>
-      <c r="L9" s="33" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
+      <c r="L9" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="35"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="32"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A10" s="4"/>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="35"/>
-      <c r="L10" s="33" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32"/>
+      <c r="L10" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="35"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="32"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A11" s="4"/>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="34"/>
-      <c r="J11" s="35"/>
-      <c r="L11" s="33" t="s">
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
+      <c r="L11" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34" t="s">
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="34"/>
-      <c r="T11" s="35"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="32"/>
     </row>
     <row r="12" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4"/>
@@ -1220,464 +1226,505 @@
       <c r="C13" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="30" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="31"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="28"/>
+      <c r="J13" s="29"/>
       <c r="L13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="M13" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="30" t="s">
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="R13" s="31"/>
+      <c r="R13" s="39"/>
       <c r="S13" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="T13" s="28"/>
+      <c r="T13" s="29"/>
     </row>
     <row r="14" spans="1:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="15"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="37"/>
     </row>
     <row r="15" spans="1:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="15"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="37"/>
     </row>
     <row r="16" spans="1:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="37"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="15"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="37"/>
     </row>
     <row r="17" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="15"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="37"/>
     </row>
     <row r="18" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="15"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="37"/>
     </row>
     <row r="19" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="15"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="37"/>
     </row>
     <row r="20" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B20" s="3"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="37"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="15"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="37"/>
     </row>
     <row r="21" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="37"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="15"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="37"/>
     </row>
     <row r="22" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="37"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="15"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="37"/>
     </row>
     <row r="23" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="37"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="15"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="37"/>
     </row>
     <row r="24" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="37"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="15"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="37"/>
     </row>
     <row r="25" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="37"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="15"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="37"/>
     </row>
     <row r="26" spans="2:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="15"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="37"/>
     </row>
     <row r="27" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="45"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="L27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="10"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="R27" s="45"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+    </row>
+    <row r="28" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="47"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="44"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="R28" s="45"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+    </row>
+    <row r="29" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="L27" s="21" t="s">
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="47"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="L29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M27" s="21"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="R27" s="18"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-    </row>
-    <row r="28" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="25"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="R28" s="18"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
-    </row>
-    <row r="29" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B29" s="21" t="s">
+      <c r="M29" s="10"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="R29" s="45"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="42"/>
+    </row>
+    <row r="30" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="41"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="44"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="R30" s="41"/>
+      <c r="S30" s="42"/>
+      <c r="T30" s="42"/>
+    </row>
+    <row r="31" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B31" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="17"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="L29" s="21" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="L31" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="R29" s="18"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-    </row>
-    <row r="30" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="25"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="R30" s="20"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-    </row>
-    <row r="31" spans="2:20" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="B31" s="21" t="s">
+      <c r="M31" s="10"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+    </row>
+    <row r="32" spans="2:20" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="L31" s="21" t="s">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="F32" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-    </row>
-    <row r="32" spans="2:20" ht="43.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
+      <c r="L32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="P32" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="B33" s="47" t="s">
+    <row r="33" spans="2:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="L33" s="47" t="s">
+      <c r="D33" s="5"/>
+      <c r="F33" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="L33" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-    </row>
-    <row r="34" spans="2:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" spans="2:20" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" spans="2:20" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="2:20" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" spans="2:20" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" spans="2:20" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" spans="2:20" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" spans="2:20" ht="11.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" spans="2:20" ht="11.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="47" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
+      <c r="N33" s="5"/>
+      <c r="P33" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="2:25" ht="19.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="5"/>
+      <c r="F34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="L34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M34" s="8"/>
+      <c r="N34" s="5"/>
+      <c r="P34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="2:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="2:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y36" s="9"/>
+    </row>
+    <row r="37" spans="2:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" spans="2:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" spans="2:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="2:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" spans="2:25" ht="11.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="45" spans="2:25" ht="11.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="47" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1692,131 +1739,7 @@
     <row r="63" ht="8.4" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="64" ht="8.4" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
-  <mergeCells count="146">
-    <mergeCell ref="N29:P30"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="D27:F28"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="D29:F30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B9:J9"/>
-    <mergeCell ref="B10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="L9:T9"/>
-    <mergeCell ref="L10:T10"/>
-    <mergeCell ref="L11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="R33:T33"/>
+  <mergeCells count="142">
     <mergeCell ref="M26:P26"/>
     <mergeCell ref="Q26:R26"/>
     <mergeCell ref="S26:T26"/>
@@ -1839,6 +1762,126 @@
     <mergeCell ref="L29:M30"/>
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="N27:P28"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="N29:P30"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="L9:T9"/>
+    <mergeCell ref="L10:T10"/>
+    <mergeCell ref="L11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B9:J9"/>
+    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="D27:F28"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="D29:F30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>